<commit_message>
Subido Historia de usuario 5 y 7
</commit_message>
<xml_diff>
--- a/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
+++ b/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Criterios de Aceptación" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="119">
   <si>
     <t xml:space="preserve">Historias de Usuario</t>
   </si>
@@ -236,6 +237,147 @@
   </si>
   <si>
     <t xml:space="preserve">Ver las facturas generadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criterios de Aceptación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID HISTORIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITULO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUANDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTONCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta inicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que existan usuarios registrados en el sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador abra la ventana de Listado de Usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un listado de todos los usuarios registrados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Búsqueda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el usuario elija un campo de búsqueda de la lista desplegable y escriba un dato en el campo la caja de texto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador presione enter en la caja de texto o de clic al botón de buscar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un listado de los usuarios que en el campo seleccionado contenga(al principio, al fin o en medio) el dato escrito en la caja de texto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Búsqueda con dato vacío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el usuario elija un campo de búsqueda de la lista desplegable y no escriba un dato en el campo la caja de texto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración inicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que no exista el archivo de configuración en la ruta del ejecutable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un usuario abra el sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá la ventana de configuración de base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que este en blanco uno o mas campos del formulario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un usuario presione el botón guardar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje avisando del primer dato faltante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conexión incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que todos los datos estén llenos pero no sean correctos(para hacer una conexión valida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje indicando la conexión incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conexión correcta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que todos los datos estén llenos y sean correctos(para hacer una conexión valida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje indicando la conexión correcta y se guardaran los datos en el archivo de configuración en la ruta del ejecutable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelación de configuración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario presiona el botón cancelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se cerrará el sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edición de la configuración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un administrador ingresado dentro del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador abra la ventana de Configuración de Base de Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá la ventana de configuración de base de datos y cargará los datos del archivo de configuración a excepción del password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guardado de configuración editada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el administrador haya escrito los datos de una conexión valida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador presione el botón guardar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje indicando la conexión correcta, se guardaran los datos en el archivo de configuración y aparecerá un mensaje de reinicio del sistema, luego se reiniciará el sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prueba de conexión incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que todos los datos estén llenos y sean incorrectos(para hacer una conexión valida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador presione el botón probar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje de conexión incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prueba de conexión correcta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparecerá un mensaje de conexión correcta</t>
   </si>
 </sst>
 </file>
@@ -245,7 +387,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -276,6 +418,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,12 +482,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,6 +504,42 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,17 +562,17 @@
   </sheetPr>
   <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,4 +1137,290 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:F17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.85"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A16"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Subido Historia de Usuario 10
</commit_message>
<xml_diff>
--- a/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
+++ b/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" state="visible" r:id="rId2"/>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">No contemplar los productos que no vendemos</t>
   </si>
   <si>
-    <t xml:space="preserve">Llevar un registro de la cantidad productos que están el inventario</t>
+    <t xml:space="preserve">Llevar un registro de la cantidad productos que están en el inventario</t>
   </si>
   <si>
     <t xml:space="preserve">Controlar la cantidad de producto existentes, la salidas y entradas</t>
@@ -387,7 +387,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -426,19 +426,43 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0079BF"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEB5A46"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9F1A"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF355263"/>
+        <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF61BD4F"/>
+        <bgColor rgb="FF99CC00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -482,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -495,6 +519,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,6 +535,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -515,7 +559,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,15 +575,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,6 +588,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0079BF"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9F1A"/>
+      <rgbColor rgb="FFEB5A46"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF61BD4F"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF355263"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -560,574 +656,608 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E37"/>
+  <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="75.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <f aca="false">A5+1</f>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="n">
+        <f aca="false">B5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <f aca="false">A6+1</f>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="n">
+        <f aca="false">B6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <f aca="false">A7+1</f>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="n">
+        <f aca="false">B7+1</f>
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <f aca="false">A8+1</f>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="n">
+        <f aca="false">B8+1</f>
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <f aca="false">A9+1</f>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="n">
+        <f aca="false">B9+1</f>
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <f aca="false">A10+1</f>
+    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="n">
+        <f aca="false">B10+1</f>
         <v>7</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <f aca="false">A11+1</f>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="n">
+        <f aca="false">B11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
-        <f aca="false">A12+1</f>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="n">
+        <f aca="false">B12+1</f>
         <v>9</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <f aca="false">A13+1</f>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4" t="n">
+        <f aca="false">B13+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <f aca="false">A14+1</f>
-        <v>11</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4" t="n">
+        <f aca="false">B14+1</f>
+        <v>11</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <f aca="false">A15+1</f>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4" t="n">
+        <f aca="false">B15+1</f>
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <f aca="false">A16+1</f>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4" t="n">
+        <f aca="false">B16+1</f>
         <v>13</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <f aca="false">A17+1</f>
+    <row r="18" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4" t="n">
+        <f aca="false">B17+1</f>
         <v>14</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
-        <f aca="false">A18+1</f>
+    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4" t="n">
+        <f aca="false">B18+1</f>
         <v>15</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <f aca="false">A19+1</f>
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8"/>
+      <c r="B20" s="4" t="n">
+        <f aca="false">B19+1</f>
         <v>16</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
-        <f aca="false">A20+1</f>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8"/>
+      <c r="B21" s="4" t="n">
+        <f aca="false">B20+1</f>
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
-        <f aca="false">A21+1</f>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
+      <c r="B22" s="4" t="n">
+        <f aca="false">B21+1</f>
         <v>18</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
-        <f aca="false">A22+1</f>
+    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8"/>
+      <c r="B23" s="4" t="n">
+        <f aca="false">B22+1</f>
         <v>19</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
-        <f aca="false">A23+1</f>
+    <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8"/>
+      <c r="B24" s="4" t="n">
+        <f aca="false">B23+1</f>
         <v>20</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
-        <f aca="false">A24+1</f>
+    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8"/>
+      <c r="B25" s="4" t="n">
+        <f aca="false">B24+1</f>
         <v>21</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
-        <f aca="false">A25+1</f>
+    <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8"/>
+      <c r="B26" s="4" t="n">
+        <f aca="false">B25+1</f>
         <v>22</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
-        <f aca="false">A26+1</f>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8"/>
+      <c r="B27" s="4" t="n">
+        <f aca="false">B26+1</f>
         <v>23</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
-        <f aca="false">A27+1</f>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8"/>
+      <c r="B28" s="4" t="n">
+        <f aca="false">B27+1</f>
         <v>24</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
-        <f aca="false">A28+1</f>
+    <row r="29" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9"/>
+      <c r="B29" s="4" t="n">
+        <f aca="false">B28+1</f>
         <v>25</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
-        <f aca="false">A29+1</f>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+      <c r="B30" s="4" t="n">
+        <f aca="false">B29+1</f>
         <v>26</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
-        <f aca="false">A30+1</f>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9"/>
+      <c r="B31" s="4" t="n">
+        <f aca="false">B30+1</f>
         <v>27</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
-        <f aca="false">A31+1</f>
+    <row r="32" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9"/>
+      <c r="B32" s="4" t="n">
+        <f aca="false">B31+1</f>
         <v>28</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
-        <f aca="false">A32+1</f>
+    <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+      <c r="B33" s="4" t="n">
+        <f aca="false">B32+1</f>
         <v>29</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
-        <f aca="false">A33+1</f>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10"/>
+      <c r="B34" s="4" t="n">
+        <f aca="false">B33+1</f>
         <v>30</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
-        <f aca="false">A34+1</f>
+    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10"/>
+      <c r="B35" s="4" t="n">
+        <f aca="false">B34+1</f>
         <v>31</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="n">
-        <f aca="false">A35+1</f>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10"/>
+      <c r="B36" s="4" t="n">
+        <f aca="false">B35+1</f>
         <v>32</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
-        <f aca="false">A36+1</f>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10"/>
+      <c r="B37" s="4" t="n">
+        <f aca="false">B36+1</f>
         <v>33</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="5" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1146,16 +1276,18 @@
   </sheetPr>
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,245 +1297,245 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="6"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="n">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="n">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="n">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="16" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="n">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="n">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="16" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="n">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="n">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="16" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="n">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="16" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9" t="n">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="16" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9" t="n">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="16" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregado Ejemplo de Selección de Objetos
</commit_message>
<xml_diff>
--- a/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
+++ b/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Modificar los datos de los productos guardados</t>
   </si>
   <si>
-    <t xml:space="preserve">Modificar en la Base de Datos</t>
+    <t xml:space="preserve">Modificar los registros en la Base de Datos</t>
   </si>
   <si>
     <t xml:space="preserve">Consultar un listado de los productos registrados</t>
@@ -658,8 +658,8 @@
   </sheetPr>
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Revert "Correcion de Errores"
This reverts commit 00b49860fb6ed4d3bfdbab933c1c9443d89b1e90.
</commit_message>
<xml_diff>
--- a/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
+++ b/Documentos/General/Realsoft_HistoriaDeUsuario_Ver1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johana\Documents\GitHub\realsoft_desarrollo\Documentos\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066D2E43-807A-4952-A11E-C553214F9767}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74D0E4B-FF5F-44AA-B77A-52C372042152}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1629,7 +1629,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J12" sqref="J12:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>